<commit_message>
updated folder names to better match product names
updated folder names to better match product names
</commit_message>
<xml_diff>
--- a/docs/build_instructions_plus.xlsx
+++ b/docs/build_instructions_plus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/607157b747fa4bbf/Documents/projects/dqmusicbox/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3402" documentId="13_ncr:1_{72E393A3-A0D9-4CED-B29E-31623CCF14F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D4256887-5F5F-4FB0-94B9-B6605B6CC537}"/>
+  <xr:revisionPtr revIDLastSave="3404" documentId="13_ncr:1_{72E393A3-A0D9-4CED-B29E-31623CCF14F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1FDAE7ED-817E-4142-8C7F-9DD335DB9A7E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>Raspberry Pi 4 Model B - 2GB RAM</t>
   </si>
   <si>
-    <t>Or order 10+ from Ponoko for @$37.89</t>
-  </si>
-  <si>
     <t>M2.5x6mm + 6mm standoffs (50 pieces)</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>Sticky back velcro strips (5 yards)</t>
+  </si>
+  <si>
+    <t>Or order 10+ from Ponoko for @$48</t>
   </si>
 </sst>
 </file>
@@ -670,7 +670,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,10 +689,10 @@
         <v>17</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -703,10 +703,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>57.92</v>
+        <v>60</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -720,7 +720,7 @@
         <v>35</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -734,12 +734,12 @@
         <v>3.95</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>9</v>
@@ -748,7 +748,7 @@
         <v>7.95</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -762,7 +762,7 @@
         <v>3.95</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -776,7 +776,7 @@
         <v>10.99</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -790,12 +790,12 @@
         <v>6.48</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>2</v>
@@ -804,7 +804,7 @@
         <v>9.99</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -818,12 +818,12 @@
         <v>9.99</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>2</v>
@@ -832,12 +832,12 @@
         <v>4.95</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>2</v>
@@ -846,7 +846,7 @@
         <v>6.34</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -860,7 +860,7 @@
         <v>17.989999999999998</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -874,7 +874,7 @@
         <v>7.99</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -888,20 +888,20 @@
         <v>4.91</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="21">
         <f>SUM(C2:C15)</f>
-        <v>188.40000000000003</v>
+        <v>190.48000000000002</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -930,7 +930,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,7 +1009,7 @@
         <v>21.5</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -1083,7 +1083,7 @@
     </row>
     <row r="8" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>25</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="9" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>25</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="10" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>25</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="11" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>25</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="12" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>2</v>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="13" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>2</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="18" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>25</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="19" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>2</v>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="20" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>25</v>
@@ -1379,12 +1379,12 @@
         <v>0.11699999999999999</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="8"/>
@@ -1395,7 +1395,7 @@
         <v>96.109999999999985</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated file names and folder names to better match product names
updated file names and folder names to better match product names
</commit_message>
<xml_diff>
--- a/docs/build_instructions_plus.xlsx
+++ b/docs/build_instructions_plus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/607157b747fa4bbf/Documents/projects/dqmusicbox/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3411" documentId="13_ncr:1_{72E393A3-A0D9-4CED-B29E-31623CCF14F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A01CC748-BA05-4627-AD06-7E0D278547A3}"/>
+  <xr:revisionPtr revIDLastSave="3413" documentId="13_ncr:1_{72E393A3-A0D9-4CED-B29E-31623CCF14F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E737CB2-C136-48CE-9AA9-C02CD595A878}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,7 +222,7 @@
     <t>Sticky back velcro strips (5 yards)</t>
   </si>
   <si>
-    <t>Or order 10+ from Ponoko for @$42.16</t>
+    <t>Or order 10+ from Ponoko for @$46.53</t>
   </si>
 </sst>
 </file>
@@ -670,7 +670,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,7 +703,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>68</v>
+        <v>69.98</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>38</v>
@@ -898,7 +898,7 @@
       <c r="B16" s="18"/>
       <c r="C16" s="21">
         <f>SUM(C2:C15)</f>
-        <v>198.48000000000002</v>
+        <v>200.46000000000004</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
updated parts list, updated Ponoko instructions - switch from SVG file to EPS file
updated parts list, updated Ponoko instructions - switch from SVG file
to EPS file
</commit_message>
<xml_diff>
--- a/docs/build_instructions_plus.xlsx
+++ b/docs/build_instructions_plus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/607157b747fa4bbf/Documents/projects/dqmusicbox/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3413" documentId="13_ncr:1_{72E393A3-A0D9-4CED-B29E-31623CCF14F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E737CB2-C136-48CE-9AA9-C02CD595A878}"/>
+  <xr:revisionPtr revIDLastSave="3418" documentId="13_ncr:1_{72E393A3-A0D9-4CED-B29E-31623CCF14F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B8D06C0B-68AB-4EF4-BCEE-1F461B9E51EA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t>KY-040 rotary encoders (knobs)</t>
   </si>
@@ -216,13 +216,16 @@
     <t>Or Amazon B07MDXBT87 or other physically small USB drive</t>
   </si>
   <si>
-    <t>This is for a large kit of sensors, you only need KY-016. Or search KY-016, but note that almost all other sellers are in China.</t>
-  </si>
-  <si>
     <t>Sticky back velcro strips (5 yards)</t>
   </si>
   <si>
     <t>Or order 10+ from Ponoko for @$46.53</t>
+  </si>
+  <si>
+    <t>Banggood</t>
+  </si>
+  <si>
+    <t>ALLOW ~3 WEEKS TO ARRIVE FROM CHINA. Due to COVID, it's hard to find these in the US. You can get it quickly from Amazon B07KJYR8K1, but costs $18.</t>
   </si>
 </sst>
 </file>
@@ -670,7 +673,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,13 +857,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C13" s="5">
-        <v>17.989999999999998</v>
+        <v>4.2699999999999996</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -898,7 +901,7 @@
       <c r="B16" s="18"/>
       <c r="C16" s="21">
         <f>SUM(C2:C15)</f>
-        <v>200.46000000000004</v>
+        <v>186.74000000000004</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>35</v>
@@ -1009,7 +1012,7 @@
         <v>21.5</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -1336,7 +1339,7 @@
     </row>
     <row r="19" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
updated parts list, including Ponoko pricing
updated parts list, including Ponoko pricing
</commit_message>
<xml_diff>
--- a/docs/build_instructions_plus.xlsx
+++ b/docs/build_instructions_plus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/607157b747fa4bbf/Documents/projects/dqmusicbox/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3418" documentId="13_ncr:1_{72E393A3-A0D9-4CED-B29E-31623CCF14F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B8D06C0B-68AB-4EF4-BCEE-1F461B9E51EA}"/>
+  <xr:revisionPtr revIDLastSave="3419" documentId="13_ncr:1_{72E393A3-A0D9-4CED-B29E-31623CCF14F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1C761BCB-4842-4F8B-8883-F48EF1E32FD6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -341,7 +341,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -386,6 +386,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -673,7 +676,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A13" sqref="A13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +856,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="24" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="11" t="s">

</xml_diff>